<commit_message>
Added inputs for variables and execute varaible check
</commit_message>
<xml_diff>
--- a/Mappe1.xlsx
+++ b/Mappe1.xlsx
@@ -476,11 +476,6 @@
           <t>Hans-Kreiling-Allee 32, 63225 Langen (Hessen)</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>1.9 km</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -493,11 +488,6 @@
           <t>Ada-Lovelace-Straße 4, 63225 Langen (Hessen)</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2.7 km</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -508,11 +498,6 @@
       <c r="B4" t="inlineStr">
         <is>
           <t>Robert-Bosch-Straße 6, 63225 Langen (Hessen)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>3.2 km</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added variables for table row file name and sheet name. Also made adress get taken with letter to match distance
</commit_message>
<xml_diff>
--- a/Mappe1.xlsx
+++ b/Mappe1.xlsx
@@ -1,38 +1,75 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ME\Privat\Projekte\Python\excel-distance-calc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B78B5F-1081-4C76-B464-3D5C7C9175D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7200" yWindow="675" windowWidth="21600" windowHeight="13185" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Adresse</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Hans-Kreiling-Allee 32, 63225 Langen (Hessen)</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Ada-Lovelace-Straße 4, 63225 Langen (Hessen)</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Robert-Bosch-Straße 6, 63225 Langen (Hessen)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -66,83 +103,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -430,78 +408,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="6.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="42.5703125" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="8.5703125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Adresse</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Distance</t>
-        </is>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Maria</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Hans-Kreiling-Allee 32, 63225 Langen (Hessen)</t>
-        </is>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Tom</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Ada-Lovelace-Straße 4, 63225 Langen (Hessen)</t>
-        </is>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Max</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Robert-Bosch-Straße 6, 63225 Langen (Hessen)</t>
-        </is>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added modes. Added Error checking. Modified Readme.md
</commit_message>
<xml_diff>
--- a/Mappe1.xlsx
+++ b/Mappe1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ME\Privat\Projekte\Python\excel-distance-calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B78B5F-1081-4C76-B464-3D5C7C9175D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FE0ED3-A87E-43B3-90A0-2B9AC5325D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="1245" windowWidth="21600" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -31,22 +31,16 @@
     <t>Distance</t>
   </si>
   <si>
+    <t>Adresse2</t>
+  </si>
+  <si>
     <t>Maria</t>
   </si>
   <si>
-    <t>Hans-Kreiling-Allee 32, 63225 Langen (Hessen)</t>
-  </si>
-  <si>
     <t>Tom</t>
   </si>
   <si>
-    <t>Ada-Lovelace-Straße 4, 63225 Langen (Hessen)</t>
-  </si>
-  <si>
     <t>Max</t>
-  </si>
-  <si>
-    <t>Robert-Bosch-Straße 6, 63225 Langen (Hessen)</t>
   </si>
 </sst>
 </file>
@@ -409,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,9 +414,11 @@
     <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,29 +428,23 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>